<commit_message>
Add RGB_TOG key to moonlander
keymap.py also supports specifying different keys for different keyboard
in a sheet cell now.
</commit_message>
<xml_diff>
--- a/mytools/keymap.xlsx
+++ b/mytools/keymap.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="135">
   <si>
     <t>BASE</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>KC_MEDIA_NEXT_TRACK</t>
+  </si>
+  <si>
+    <t>{"moonlander": "RGB_TOG", "ergodox_ez": "x"}</t>
   </si>
   <si>
     <t>KC_AUDIO_VOL_DOWN</t>
@@ -438,7 +441,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +474,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF7F6000"/>
         <bgColor rgb="FF7F6000"/>
       </patternFill>
@@ -482,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -501,10 +510,13 @@
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -751,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
@@ -763,16 +775,16 @@
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -780,19 +792,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>1</v>
@@ -801,19 +813,19 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>1</v>
@@ -821,81 +833,81 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>1</v>
@@ -903,7 +915,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -912,1118 +924,1118 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="J7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
       <c r="G8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
       <c r="G16" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
       <c r="G24" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="N30" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
+        <v>104</v>
+      </c>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J39" s="7" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
     </row>
     <row r="40">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
       <c r="G40" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42">
@@ -2215,10 +2227,10 @@
       <c r="F46" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="5" t="s">
+      <c r="G46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I46" s="5" t="s">
@@ -2241,44 +2253,44 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
       <c r="G48" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="42">

</xml_diff>